<commit_message>
edit specification in request and response
</commit_message>
<xml_diff>
--- a/src/main/resources/menName.xlsx
+++ b/src/main/resources/menName.xlsx
@@ -8,8 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="list-1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="list-2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="male-names" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="female-names" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,14 +21,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
-  <si>
-    <t xml:space="preserve">id</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+  <si>
+    <t xml:space="preserve">count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gender</t>
   </si>
   <si>
     <t xml:space="preserve">name</t>
   </si>
   <si>
+    <t xml:space="preserve">probability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">male</t>
+  </si>
+  <si>
     <t xml:space="preserve">Albert</t>
   </si>
   <si>
@@ -59,10 +68,16 @@
     <t xml:space="preserve">Greg</t>
   </si>
   <si>
+    <t xml:space="preserve">female</t>
+  </si>
+  <si>
     <t xml:space="preserve">Alice</t>
   </si>
   <si>
     <t xml:space="preserve">Marry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.98</t>
   </si>
 </sst>
 </file>
@@ -72,7 +87,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -93,6 +108,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -144,17 +166,37 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -174,101 +216,240 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:AMJ11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="3:3 D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="1" style="1" width="11.57"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
+    <row r="2" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="n">
+        <v>206600</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="D2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AMD2" s="0"/>
+      <c r="AME2" s="0"/>
+      <c r="AMF2" s="0"/>
+      <c r="AMG2" s="0"/>
+      <c r="AMH2" s="0"/>
+      <c r="AMI2" s="0"/>
+      <c r="AMJ2" s="0"/>
+    </row>
+    <row r="3" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="n">
+        <v>531783</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="D3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AMD3" s="0"/>
+      <c r="AME3" s="0"/>
+      <c r="AMF3" s="0"/>
+      <c r="AMG3" s="0"/>
+      <c r="AMH3" s="0"/>
+      <c r="AMI3" s="0"/>
+      <c r="AMJ3" s="0"/>
+    </row>
+    <row r="4" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="n">
+        <v>2274744</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="D4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AMD4" s="0"/>
+      <c r="AME4" s="0"/>
+      <c r="AMF4" s="0"/>
+      <c r="AMG4" s="0"/>
+      <c r="AMH4" s="0"/>
+      <c r="AMI4" s="0"/>
+      <c r="AMJ4" s="0"/>
+    </row>
+    <row r="5" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="n">
+        <v>177229</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="D5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AMD5" s="0"/>
+      <c r="AME5" s="0"/>
+      <c r="AMF5" s="0"/>
+      <c r="AMG5" s="0"/>
+      <c r="AMH5" s="0"/>
+      <c r="AMI5" s="0"/>
+      <c r="AMJ5" s="0"/>
+    </row>
+    <row r="6" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="n">
+        <v>757890</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="D6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AMD6" s="0"/>
+      <c r="AME6" s="0"/>
+      <c r="AMF6" s="0"/>
+      <c r="AMG6" s="0"/>
+      <c r="AMH6" s="0"/>
+      <c r="AMI6" s="0"/>
+      <c r="AMJ6" s="0"/>
+    </row>
+    <row r="7" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="n">
+        <v>472543</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="D7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AMD7" s="0"/>
+      <c r="AME7" s="0"/>
+      <c r="AMF7" s="0"/>
+      <c r="AMG7" s="0"/>
+      <c r="AMH7" s="0"/>
+      <c r="AMI7" s="0"/>
+      <c r="AMJ7" s="0"/>
+    </row>
+    <row r="8" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="n">
+        <v>2087284</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="D8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AMD8" s="0"/>
+      <c r="AME8" s="0"/>
+      <c r="AMF8" s="0"/>
+      <c r="AMG8" s="0"/>
+      <c r="AMH8" s="0"/>
+      <c r="AMI8" s="0"/>
+      <c r="AMJ8" s="0"/>
+    </row>
+    <row r="9" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="n">
+        <v>97618</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AMD9" s="0"/>
+      <c r="AME9" s="0"/>
+      <c r="AMF9" s="0"/>
+      <c r="AMG9" s="0"/>
+      <c r="AMH9" s="0"/>
+      <c r="AMI9" s="0"/>
+      <c r="AMJ9" s="0"/>
+    </row>
+    <row r="10" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="n">
+        <v>771585</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AMD10" s="0"/>
+      <c r="AME10" s="0"/>
+      <c r="AMF10" s="0"/>
+      <c r="AMG10" s="0"/>
+      <c r="AMH10" s="0"/>
+      <c r="AMI10" s="0"/>
+      <c r="AMJ10" s="0"/>
+    </row>
+    <row r="11" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="n">
+        <v>345494</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AMD11" s="0"/>
+      <c r="AME11" s="0"/>
+      <c r="AMF11" s="0"/>
+      <c r="AMG11" s="0"/>
+      <c r="AMH11" s="0"/>
+      <c r="AMI11" s="0"/>
+      <c r="AMJ11" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -286,10 +467,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M8" activeCellId="0" sqref="M8"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="3:3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -301,21 +482,39 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>13</v>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="n">
+        <v>277052</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="n">
+        <v>6650</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>